<commit_message>
the download button logic needs to be implemented for complete functionality
</commit_message>
<xml_diff>
--- a/web/web_allocation_project/output.xlsx
+++ b/web/web_allocation_project/output.xlsx
@@ -11934,22 +11934,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1, 2, 4, 7, 8, 10</t>
+          <t>1, 2, 4, 7, 8, 9</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6</t>
+          <t>1, 2, 3, 4, 5, 7</t>
         </is>
       </c>
       <c r="G2" t="n">
         <v>6</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="J2" t="n">
-        <v>100</v>
+        <v>97.01000000000001</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -11989,7 +11989,7 @@
         <v>100</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>2.99</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -12078,19 +12078,19 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2, 4, 6, 7, 10</t>
+          <t>4, 6, 7, 8, 10</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>4, 1, 5, 2, 3</t>
+          <t>1, 5, 2, 7, 3</t>
         </is>
       </c>
       <c r="G6" t="n">
         <v>5</v>
       </c>
       <c r="H6" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7">
@@ -12110,19 +12110,19 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1, 3, 4, 7, 8</t>
+          <t>1, 4, 7, 8, 9</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4, 5, 3, 2, 1</t>
+          <t>4, 3, 2, 1, 7</t>
         </is>
       </c>
       <c r="G7" t="n">
         <v>5</v>
       </c>
       <c r="H7" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
@@ -12174,12 +12174,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -12206,12 +12206,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -12238,19 +12238,19 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2, 3, 4, 5, 6, 10</t>
+          <t>2, 4, 5, 6, 9, 10</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2, 6, 1, 3, 4, 5</t>
+          <t>2, 1, 3, 4, 7, 5</t>
         </is>
       </c>
       <c r="G11" t="n">
         <v>6</v>
       </c>
       <c r="H11" t="n">
-        <v>100</v>
+        <v>83.33333333333334</v>
       </c>
     </row>
     <row r="12">
@@ -12270,12 +12270,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2, 7, 9, 10</t>
+          <t>7, 8, 9, 10</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>3, 1, 2, 4</t>
+          <t>1, 6, 2, 4</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -12334,12 +12334,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -12398,19 +12398,19 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2, 4, 5, 6, 9, 10</t>
+          <t>4, 5, 6, 8, 9, 10</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>6, 3, 5, 4, 2, 1</t>
+          <t>3, 5, 4, 8, 2, 1</t>
         </is>
       </c>
       <c r="G16" t="n">
         <v>6</v>
       </c>
       <c r="H16" t="n">
-        <v>100</v>
+        <v>83.33333333333334</v>
       </c>
     </row>
     <row r="17">
@@ -12430,12 +12430,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1, 2, 4</t>
+          <t>1, 4, 8</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>3, 1, 2</t>
+          <t>3, 2, 5</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -12462,12 +12462,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3, 4</t>
+          <t>3, 5</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>1, 2</t>
+          <t>1, 3</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -12526,12 +12526,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4</t>
+          <t>1, 2, 4, 6</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2, 1, 4, 3</t>
+          <t>2, 1, 3, 5</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -12590,12 +12590,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2, 3, 4, 10</t>
+          <t>3, 5, 9, 10</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>3, 1, 4, 2</t>
+          <t>1, 6, 5, 2</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -12686,12 +12686,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3, 4</t>
+          <t>3, 5</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>1, 2</t>
+          <t>1, 3</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -12750,12 +12750,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1, 2, 7</t>
+          <t>1, 6, 7</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>1, 2, 3</t>
+          <t>1, 5, 3</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -12974,12 +12974,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2, 3</t>
+          <t>3, 9</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>1, 2</t>
+          <t>2, 4</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -13134,19 +13134,19 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 6, 10</t>
+          <t>1, 2, 4, 6, 9, 10</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>3, 1, 6, 2, 4, 5</t>
+          <t>3, 1, 2, 4, 8, 5</t>
         </is>
       </c>
       <c r="G39" t="n">
         <v>6</v>
       </c>
       <c r="H39" t="n">
-        <v>100</v>
+        <v>83.33333333333334</v>
       </c>
     </row>
     <row r="40">
@@ -13230,19 +13230,19 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2, 3, 4, 6, 7, 10</t>
+          <t>2, 3, 4, 6, 8, 10</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2, 3, 1, 4, 6, 5</t>
+          <t>2, 3, 1, 4, 7, 5</t>
         </is>
       </c>
       <c r="G42" t="n">
         <v>6</v>
       </c>
       <c r="H42" t="n">
-        <v>100</v>
+        <v>83.33333333333334</v>
       </c>
     </row>
     <row r="43">
@@ -13262,12 +13262,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2, 4, 5, 10</t>
+          <t>4, 5, 6, 10</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>3, 1, 2, 4</t>
+          <t>1, 2, 5, 4</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -13326,19 +13326,19 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1, 2, 4, 7, 8, 10</t>
+          <t>1, 2, 4, 7, 8, 9</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>1, 2, 3, 5, 4, 6</t>
+          <t>1, 2, 3, 5, 4, 7</t>
         </is>
       </c>
       <c r="G45" t="n">
         <v>6</v>
       </c>
       <c r="H45" t="n">
-        <v>100</v>
+        <v>83.33333333333334</v>
       </c>
     </row>
     <row r="46">
@@ -13358,12 +13358,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1, 2</t>
+          <t>1, 3</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2, 1</t>
+          <t>2, 3</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -13454,19 +13454,19 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 7, 8</t>
+          <t>1, 2, 4, 5, 7, 8</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1, 2, 6, 5, 3, 4</t>
+          <t>1, 2, 5, 7, 3, 4</t>
         </is>
       </c>
       <c r="G49" t="n">
         <v>6</v>
       </c>
       <c r="H49" t="n">
-        <v>100</v>
+        <v>83.33333333333334</v>
       </c>
     </row>
     <row r="50">
@@ -13486,12 +13486,12 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2, 3, 6, 7</t>
+          <t>2, 6, 7, 9</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>1, 4, 3, 2</t>
+          <t>1, 3, 2, 6</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -13518,12 +13518,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2, 4, 6, 7</t>
+          <t>2, 4, 6, 9</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4</t>
+          <t>1, 2, 3, 6</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -13550,19 +13550,19 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1, 2, 3, 7, 8</t>
+          <t>1, 3, 7, 8, 9</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2, 3, 1, 5, 4</t>
+          <t>2, 1, 5, 4, 7</t>
         </is>
       </c>
       <c r="G52" t="n">
         <v>5</v>
       </c>
       <c r="H52" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53">
@@ -13614,12 +13614,12 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>4, 9, 10</t>
+          <t>6, 9, 10</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>3, 2, 1</t>
+          <t>4, 2, 1</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -13678,12 +13678,12 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2, 4, 6, 10</t>
+          <t>4, 6, 8, 10</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2, 4, 3, 1</t>
+          <t>4, 3, 6, 1</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -13710,12 +13710,12 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2, 5, 6, 10</t>
+          <t>2, 5, 6, 9</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>1, 3, 2, 4</t>
+          <t>1, 3, 2, 5</t>
         </is>
       </c>
       <c r="G57" t="n">
@@ -13806,12 +13806,12 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>3, 7</t>
+          <t>3, 8</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>1, 2</t>
+          <t>1, 4</t>
         </is>
       </c>
       <c r="G60" t="n">

</xml_diff>